<commit_message>
Update the get/put subframe functions
</commit_message>
<xml_diff>
--- a/adjust_image_params.xlsx
+++ b/adjust_image_params.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A04B4B4-41DC-4752-9502-682BFC0286FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0F4F4C-C4E5-4653-B987-81A5B8F1AAC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="-110" windowWidth="37480" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="0" windowWidth="20500" windowHeight="10190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -686,7 +686,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="7">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:2">

</xml_diff>

<commit_message>
Add support for mono camera
</commit_message>
<xml_diff>
--- a/adjust_image_params.xlsx
+++ b/adjust_image_params.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9944562F-BF6D-42FD-86B5-E1181D4B3DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F55A10-8592-45E5-86A2-BF36DEF4EB61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1030" yWindow="-110" windowWidth="37480" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7630" yWindow="-110" windowWidth="37480" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>color</t>
   </si>
@@ -148,6 +148,36 @@
   <si>
     <t>/home/hao/astro/raw/2022-07-07_21_27_18Z/output/</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>叠加模式</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LRGB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RGB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LHSO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HSO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>color</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用直方图均衡化</t>
+  </si>
+  <si>
+    <t>彩色相机照片使用color，黑白相机配滤镜照片使用其余。</t>
   </si>
 </sst>
 </file>
@@ -155,13 +185,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -169,13 +199,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -227,7 +257,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -238,10 +268,10 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -530,19 +560,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="34.08203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.08984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.1796875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="3" customFormat="1" hidden="1">
       <c r="A1" s="4">
         <v>1</v>
       </c>
@@ -550,7 +580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="3" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="3" customFormat="1" ht="18.5">
       <c r="A2" s="11" t="s">
         <v>28</v>
       </c>
@@ -558,7 +588,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="3" customFormat="1">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -566,7 +596,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="3" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
@@ -574,11 +604,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -586,7 +616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -594,7 +624,7 @@
         <v>65535</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -602,11 +632,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -614,7 +644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -622,11 +652,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -634,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -642,11 +672,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" s="5"/>
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -654,7 +684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
@@ -662,11 +692,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
@@ -674,7 +704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20" s="10" t="s">
         <v>14</v>
       </c>
@@ -682,7 +712,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
@@ -690,7 +720,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
@@ -698,11 +728,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23" s="5"/>
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24" s="5" t="s">
         <v>30</v>
       </c>
@@ -710,7 +740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25" s="5" t="s">
         <v>31</v>
       </c>
@@ -718,7 +748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
@@ -726,11 +756,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27" s="5"/>
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28" s="5" t="s">
         <v>33</v>
       </c>
@@ -738,7 +768,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="A29" s="5" t="s">
         <v>34</v>
       </c>
@@ -746,7 +776,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2">
       <c r="A30" s="5" t="s">
         <v>35</v>
       </c>
@@ -754,11 +784,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2">
       <c r="A31" s="5"/>
       <c r="B31" s="9"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2">
       <c r="A32" s="5" t="s">
         <v>39</v>
       </c>
@@ -766,11 +796,34 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4">
       <c r="A33" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="5"/>
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -806,18 +859,24 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D12ED5D5-DB7D-4F2A-9A6A-33B84B8DCE7A}">
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B24:B26 B10:B17 B32:B33 D13:D14</xm:sqref>
+          <xm:sqref>B24:B26 B10:B17 D13:D14 B32:B34 B36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8B448712-EE79-4087-80FF-23B5610E47F3}">
           <x14:formula1>
             <xm:f>Sheet2!$E$1:$E$4</xm:f>
           </x14:formula1>
           <xm:sqref>B8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9ABDEB00-DD78-4DD1-B92F-55B166ADD185}">
+          <x14:formula1>
+            <xm:f>Sheet2!$F$1:$F$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>B35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -827,18 +886,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFA129CA-FAFF-4C45-9C55-7F069F386FAE}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -854,8 +913,11 @@
       <c r="E1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -871,19 +933,34 @@
       <c r="E2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="E3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="E4" t="s">
         <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="F5" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix some bugs of multi-channel processing
</commit_message>
<xml_diff>
--- a/adjust_image_params.xlsx
+++ b/adjust_image_params.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F55A10-8592-45E5-86A2-BF36DEF4EB61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2483B4D2-0D3C-4305-BF93-847D5A7E275F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7630" yWindow="-110" windowWidth="37480" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1030" yWindow="-110" windowWidth="37480" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>color</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>彩色相机照片使用color，黑白相机配滤镜照片使用其余。</t>
+  </si>
+  <si>
+    <t>HSO</t>
+  </si>
+  <si>
+    <t>通道名格式（紧邻前缀）</t>
+  </si>
+  <si>
+    <t>_Bin2_</t>
   </si>
 </sst>
 </file>
@@ -185,13 +194,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -199,13 +208,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -257,7 +266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -268,10 +277,10 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -560,19 +569,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.08203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.1640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" hidden="1">
+    <row r="1" spans="1:2" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4">
         <v>1</v>
       </c>
@@ -580,7 +589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="3" customFormat="1" ht="18.5">
+    <row r="2" spans="1:2" s="3" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>28</v>
       </c>
@@ -588,7 +597,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="3" customFormat="1">
+    <row r="3" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -596,7 +605,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="3" customFormat="1">
+    <row r="4" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
@@ -604,11 +613,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -616,7 +625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -624,7 +633,7 @@
         <v>65535</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -632,11 +641,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -644,7 +653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -652,11 +661,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -664,7 +673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -672,11 +681,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -684,7 +693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
@@ -692,11 +701,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
@@ -704,7 +713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>14</v>
       </c>
@@ -712,7 +721,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
@@ -720,7 +729,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
@@ -728,11 +737,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>30</v>
       </c>
@@ -740,7 +749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>31</v>
       </c>
@@ -748,7 +757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
@@ -756,11 +765,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>33</v>
       </c>
@@ -768,7 +777,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>34</v>
       </c>
@@ -776,7 +785,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>35</v>
       </c>
@@ -784,11 +793,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="9"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>39</v>
       </c>
@@ -796,7 +805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>40</v>
       </c>
@@ -804,27 +813,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="7"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="5"/>
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -892,12 +913,12 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="13.36328125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -917,7 +938,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -937,7 +958,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
         <v>24</v>
       </c>
@@ -945,7 +966,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
         <v>25</v>
       </c>
@@ -953,7 +974,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F5" t="s">
         <v>46</v>
       </c>

</xml_diff>